<commit_message>
Changed Routing of 9V line, added more documentation
</commit_message>
<xml_diff>
--- a/Documentation/GainChart.xlsx
+++ b/Documentation/GainChart.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DamianL\Desktop\Radar Project\hardware\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="10540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>MAX 2752 (VCO)</t>
   </si>
@@ -110,12 +115,27 @@
   </si>
   <si>
     <t>GALI -2+ and 4P Filter</t>
+  </si>
+  <si>
+    <t>The Amplifier and Filter were simulated together</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Band Stop</t>
+  </si>
+  <si>
+    <t>-9dB &amp; -12dB</t>
+  </si>
+  <si>
+    <t>Insetrion Loss &amp; Single Pole Filter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -202,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -417,6 +437,32 @@
       <left/>
       <right style="thin">
         <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
@@ -431,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -466,13 +512,55 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -487,48 +575,28 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,18 +904,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N6" sqref="M6:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -858,65 +926,65 @@
     <col min="6" max="6" width="4.6328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.6328125" customWidth="1"/>
-    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.36328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.7265625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.6328125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="4.1796875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="4.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.5">
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="G4" s="35" t="s">
+      <c r="D4" s="38"/>
+      <c r="G4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="K4" s="35" t="s">
+      <c r="H4" s="38"/>
+      <c r="K4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="36"/>
-      <c r="O4" s="35" t="s">
+      <c r="L4" s="38"/>
+      <c r="O4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="36"/>
-      <c r="S4" s="35" t="s">
+      <c r="P4" s="38"/>
+      <c r="S4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="T4" s="36"/>
-      <c r="W4" s="35" t="s">
+      <c r="T4" s="38"/>
+      <c r="W4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="X4" s="36"/>
+      <c r="X4" s="38"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
@@ -928,40 +996,35 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="7">
-        <f>E6+G5</f>
-        <v>7</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
       <c r="K5" s="6">
-        <v>-12</v>
+        <v>-16.5</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="M5" s="7">
-        <f>I5+K5</f>
-        <v>-5</v>
+        <f>I6+K5</f>
+        <v>-7.5</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="O5" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Q5" s="7">
         <f>M5+O5</f>
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>3</v>
@@ -974,15 +1037,15 @@
       </c>
       <c r="U5" s="10">
         <f>Q5+S5</f>
-        <v>1.9</v>
+        <v>1.4</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="W5" s="37" t="s">
+      <c r="W5" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="38"/>
+      <c r="X5" s="52"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
@@ -999,12 +1062,24 @@
       </c>
       <c r="G6" s="41"/>
       <c r="H6" s="42"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="41"/>
+      <c r="I6" s="18">
+        <f>E6+G5</f>
+        <v>9</v>
+      </c>
+      <c r="J6" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="65" t="s">
+        <v>33</v>
+      </c>
       <c r="L6" s="42"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
+      <c r="M6" s="64">
+        <f>M5-9-12</f>
+        <v>-28.5</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="O6" s="41"/>
       <c r="P6" s="42"/>
       <c r="Q6" s="11"/>
@@ -1013,10 +1088,10 @@
       <c r="T6" s="42"/>
       <c r="U6" s="11"/>
       <c r="V6" s="11"/>
-      <c r="W6" s="39" t="s">
+      <c r="W6" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="X6" s="40"/>
+      <c r="X6" s="54"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
@@ -1043,143 +1118,145 @@
       <c r="T7" s="16"/>
       <c r="U7" s="14"/>
       <c r="V7" s="14"/>
-      <c r="W7" s="51"/>
-      <c r="X7" s="52"/>
-    </row>
-    <row r="8" spans="1:24" ht="21" x14ac:dyDescent="0.5">
-      <c r="C8" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="34"/>
-      <c r="V8" s="34"/>
+      <c r="W7" s="39"/>
+      <c r="X7" s="40"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A8" s="66"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="66"/>
+      <c r="R8" s="66"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="66"/>
+      <c r="V8" s="66"/>
       <c r="W8" s="34"/>
       <c r="X8" s="34"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="G11" s="35" t="s">
+    <row r="9" spans="1:24" ht="21" x14ac:dyDescent="0.5">
+      <c r="C9" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="44"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="44"/>
+      <c r="U9" s="44"/>
+      <c r="V9" s="44"/>
+      <c r="W9" s="44"/>
+      <c r="X9" s="44"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="C12" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="38"/>
+      <c r="G12" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="36"/>
-      <c r="K11" s="35" t="s">
+      <c r="H12" s="38"/>
+      <c r="K12" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="36"/>
-      <c r="O11" s="35" t="s">
+      <c r="L12" s="38"/>
+      <c r="O12" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="P11" s="36"/>
-      <c r="S11" s="44" t="s">
+      <c r="P12" s="38"/>
+      <c r="S12" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="T11" s="45"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="26"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20">
-        <f>U5</f>
-        <v>1.9</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="6">
-        <v>11.9</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="7">
-        <f>E12+G12</f>
-        <v>13.8</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M12" s="7" t="e">
-        <f>I12+K12</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="O12" s="6">
-        <v>10</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q12" s="7" t="e">
-        <f>M12+O12</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="S12" s="44"/>
-      <c r="T12" s="48"/>
+      <c r="T12" s="46"/>
       <c r="U12" s="27"/>
       <c r="V12" s="26"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="25"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="41">
-        <v>-3.6</v>
-      </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="46"/>
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="52"/>
+      <c r="E13" s="20">
+        <f>U5</f>
+        <v>1.4</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="6">
+        <v>11.9</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="7">
+        <f>E13+G13</f>
+        <v>13.3</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" s="7">
+        <f>I13+K13</f>
+        <v>13.3</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" s="6">
+        <v>0</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="7">
+        <f>M13+O13</f>
+        <v>13.3</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="S13" s="45"/>
       <c r="T13" s="47"/>
       <c r="U13" s="27"/>
       <c r="V13" s="26"/>
@@ -1187,296 +1264,313 @@
       <c r="X13" s="25"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="23">
-        <v>-58.5</v>
-      </c>
-      <c r="P14" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="32"/>
+      <c r="A14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="41">
+        <v>-3.6</v>
+      </c>
+      <c r="H14" s="42"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="50"/>
       <c r="U14" s="27"/>
       <c r="V14" s="26"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-    </row>
-    <row r="17" spans="1:24" ht="21" x14ac:dyDescent="0.5">
-      <c r="C17" s="34" t="s">
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A15" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="23">
+        <v>-58.5</v>
+      </c>
+      <c r="P15" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="G16" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="55"/>
+    </row>
+    <row r="18" spans="1:24" ht="21" x14ac:dyDescent="0.5">
+      <c r="C18" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="34"/>
-      <c r="T17" s="34"/>
-      <c r="U17" s="34"/>
-      <c r="V17" s="34"/>
-      <c r="W17" s="34"/>
-      <c r="X17" s="34"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="C20" s="44" t="s">
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="44"/>
+      <c r="Q18" s="44"/>
+      <c r="R18" s="44"/>
+      <c r="S18" s="44"/>
+      <c r="T18" s="44"/>
+      <c r="U18" s="44"/>
+      <c r="V18" s="44"/>
+      <c r="W18" s="44"/>
+      <c r="X18" s="44"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="C21" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="45"/>
-      <c r="G20" s="35" t="s">
+      <c r="D21" s="47"/>
+      <c r="G21" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="36"/>
-      <c r="K20" s="35" t="s">
+      <c r="H21" s="38"/>
+      <c r="K21" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="L20" s="36"/>
-      <c r="O20" s="35" t="s">
+      <c r="L21" s="38"/>
+      <c r="O21" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="P20" s="36"/>
-      <c r="S20" s="35" t="s">
+      <c r="P21" s="38"/>
+      <c r="S21" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="T20" s="36"/>
-      <c r="W20" s="35" t="s">
+      <c r="T21" s="38"/>
+      <c r="W21" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="X20" s="36"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+      <c r="X21" s="38"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="6" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="6">
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="6">
         <v>11.8</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="L22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="6">
-        <v>10</v>
-      </c>
-      <c r="P21" s="6" t="s">
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="6">
+        <v>-10</v>
+      </c>
+      <c r="P22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="51" t="s">
+      <c r="Q22" s="61"/>
+      <c r="R22" s="62"/>
+      <c r="S22" s="58"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="60"/>
+      <c r="V22" s="60"/>
+      <c r="W22" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="X21" s="52"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+      <c r="X22" s="40"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="41"/>
-      <c r="T22" s="42"/>
-      <c r="U22" s="22"/>
-      <c r="V22" s="22"/>
-      <c r="W22" s="2">
+      <c r="B23" s="11"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="48"/>
+      <c r="T23" s="59"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="2">
         <v>1000</v>
       </c>
-      <c r="X22" s="3" t="s">
+      <c r="X23" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A24" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="21"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="24"/>
-      <c r="U23" s="21"/>
-      <c r="V23" s="21"/>
-      <c r="W23" s="51" t="s">
+      <c r="B24" s="21"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="T24" s="57"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="X23" s="52"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="29"/>
+      <c r="X24" s="40"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="G25" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
       <c r="M25" s="28"/>
       <c r="N25" s="28"/>
       <c r="O25" s="29"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="G26" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="53"/>
-      <c r="I26" s="1">
-        <f>U5</f>
-        <v>1.9</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K26" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L26" s="36"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
       <c r="O26" s="29"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="G27" s="49" t="s">
+      <c r="G27" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="43"/>
+      <c r="I27" s="1">
+        <f>U5</f>
+        <v>1.4</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="L27" s="38"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="29"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="G28" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="50"/>
-      <c r="K27" s="6">
+      <c r="H28" s="36"/>
+      <c r="K28" s="6">
         <v>10</v>
       </c>
-      <c r="L27" s="6" t="s">
+      <c r="L28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M27" s="1">
-        <f>K27+I26</f>
-        <v>11.9</v>
-      </c>
-      <c r="N27" s="1" t="s">
+      <c r="M28" s="1">
+        <f>K28+I27</f>
+        <v>11.4</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O27" s="30"/>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="G28" s="49"/>
-      <c r="H28" s="50"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="42"/>
+      <c r="O28" s="30"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="G29" s="49"/>
-      <c r="H29" s="50"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="24"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="36"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="42"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="G30" s="35"/>
+      <c r="H30" s="36"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="W20:X20"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="C17:X17"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="C8:X8"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="S6:T6"/>
+  <mergeCells count="52">
+    <mergeCell ref="G25:L25"/>
+    <mergeCell ref="G16:L16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="S24:T24"/>
     <mergeCell ref="C1:X1"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="G4:H4"/>
@@ -1484,6 +1578,45 @@
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="W4:X4"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="C9:X9"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="C18:X18"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>